<commit_message>
Add consecutive locked nucleic acid calculation
</commit_message>
<xml_diff>
--- a/vignettes/Tables.xlsx
+++ b/vignettes/Tables.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\J. Aravind\Dropbox\R packages\rmelting\vignettes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Dropbox\R packages\rmelting\vignettes\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F69D13E-4ACF-4DD7-95DC-F60F8AB8889E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" firstSheet="3" activeTab="3"/>
+    <workbookView xWindow="15540" yWindow="345" windowWidth="13260" windowHeight="15255" firstSheet="16" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Approx.methods" sheetId="1" r:id="rId1"/>
@@ -27,23 +28,25 @@
     <sheet name="inosine.methods" sheetId="14" r:id="rId13"/>
     <sheet name="hydroxyadenine.methods" sheetId="15" r:id="rId14"/>
     <sheet name="azobenzenes.methods" sheetId="16" r:id="rId15"/>
-    <sheet name="locked.methods" sheetId="17" r:id="rId16"/>
-    <sheet name="na.correction" sheetId="18" r:id="rId17"/>
-    <sheet name="mg.correction" sheetId="19" r:id="rId18"/>
-    <sheet name="NaMg.correction" sheetId="20" r:id="rId19"/>
-    <sheet name="Naeq.methods" sheetId="21" r:id="rId20"/>
-    <sheet name="DMSO.methods" sheetId="22" r:id="rId21"/>
-    <sheet name="formamide.methods" sheetId="23" r:id="rId22"/>
-    <sheet name="commands" sheetId="7" r:id="rId23"/>
-    <sheet name="Models summary" sheetId="25" r:id="rId24"/>
-    <sheet name="Correction" sheetId="26" r:id="rId25"/>
-    <sheet name="IUPAC" sheetId="24" r:id="rId26"/>
-    <sheet name="MELTING" sheetId="27" r:id="rId27"/>
-    <sheet name="HybType" sheetId="28" r:id="rId28"/>
+    <sheet name="single.locked.methods" sheetId="17" r:id="rId16"/>
+    <sheet name="consq.locked.methods" sheetId="29" r:id="rId17"/>
+    <sheet name="consq.locked.SMM.methods" sheetId="30" r:id="rId18"/>
+    <sheet name="na.correction" sheetId="18" r:id="rId19"/>
+    <sheet name="mg.correction" sheetId="19" r:id="rId20"/>
+    <sheet name="NaMg.correction" sheetId="20" r:id="rId21"/>
+    <sheet name="Naeq.methods" sheetId="21" r:id="rId22"/>
+    <sheet name="DMSO.methods" sheetId="22" r:id="rId23"/>
+    <sheet name="formamide.methods" sheetId="23" r:id="rId24"/>
+    <sheet name="commands" sheetId="7" r:id="rId25"/>
+    <sheet name="Models summary" sheetId="25" r:id="rId26"/>
+    <sheet name="Correction" sheetId="26" r:id="rId27"/>
+    <sheet name="IUPAC" sheetId="24" r:id="rId28"/>
+    <sheet name="MELTING" sheetId="27" r:id="rId29"/>
+    <sheet name="HybType" sheetId="28" r:id="rId30"/>
   </sheets>
   <definedNames>
-    <definedName name="SECTION000511000000000000000" localSheetId="23">'Models summary'!$B$12</definedName>
-    <definedName name="SECTION00054100000000000000" localSheetId="24">Correction!$B$3</definedName>
+    <definedName name="SECTION000511000000000000000" localSheetId="25">'Models summary'!$B$12</definedName>
+    <definedName name="SECTION00054100000000000000" localSheetId="26">Correction!$B$3</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
   <extLst>
@@ -55,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="754" uniqueCount="338">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="783" uniqueCount="346">
   <si>
     <t>ahs01</t>
   </si>
@@ -1069,12 +1072,36 @@
   </si>
   <si>
     <t>wat11</t>
+  </si>
+  <si>
+    <t>owc11</t>
+  </si>
+  <si>
+    <t>[@owczarzy_stability_2011]</t>
+  </si>
+  <si>
+    <t>tanLck</t>
+  </si>
+  <si>
+    <t>sinMMLck</t>
+  </si>
+  <si>
+    <t>Remarks1</t>
+  </si>
+  <si>
+    <t>Remarks2</t>
+  </si>
+  <si>
+    <t>method.consecutive.locked</t>
+  </si>
+  <si>
+    <t>method.consecutive.locked.singleMM</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="6">
     <font>
       <sz val="11"/>
@@ -1464,7 +1491,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1632,7 +1659,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1720,7 +1747,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1786,7 +1813,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1835,7 +1862,7 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1901,7 +1928,7 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1950,7 +1977,7 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1999,11 +2026,11 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2029,6 +2056,64 @@
       <c r="A2" t="s">
         <v>130</v>
       </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>338</v>
+      </c>
+      <c r="B3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" t="s">
+        <v>339</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1D3B3C4-D912-4CE0-BFFC-FB974D8ADB40}">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K26" sqref="K26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>338</v>
+      </c>
       <c r="B2" t="s">
         <v>28</v>
       </c>
@@ -2036,7 +2121,54 @@
         <v>10</v>
       </c>
       <c r="E2" t="s">
-        <v>157</v>
+        <v>339</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F866593-5C74-4185-BBF7-E9942CD7540B}">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q33" sqref="Q33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>338</v>
+      </c>
+      <c r="B2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
+        <v>339</v>
       </c>
     </row>
   </sheetData>
@@ -2044,8 +2176,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2267,154 +2399,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" s="1" t="s">
-        <v>334</v>
-      </c>
-      <c r="B1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" t="s">
-        <v>192</v>
-      </c>
-      <c r="B2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" t="s">
-        <v>173</v>
-      </c>
-      <c r="E2" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" t="s">
-        <v>142</v>
-      </c>
-      <c r="C3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" t="s">
-        <v>174</v>
-      </c>
-      <c r="E3" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" t="s">
-        <v>143</v>
-      </c>
-      <c r="B4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C4" t="s">
-        <v>191</v>
-      </c>
-      <c r="D4" t="s">
-        <v>175</v>
-      </c>
-      <c r="E4" t="s">
-        <v>118</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="4" max="4" width="31.28515625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" s="1" t="s">
-        <v>334</v>
-      </c>
-      <c r="B1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="30">
-      <c r="A2" t="s">
-        <v>193</v>
-      </c>
-      <c r="B2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="E2" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="75">
-      <c r="A3" t="s">
-        <v>144</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>212</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="E3" t="s">
-        <v>118</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2621,7 +2607,153 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="B1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>192</v>
+      </c>
+      <c r="B2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
+        <v>173</v>
+      </c>
+      <c r="E2" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>142</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
+        <v>174</v>
+      </c>
+      <c r="E3" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>143</v>
+      </c>
+      <c r="B4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" t="s">
+        <v>191</v>
+      </c>
+      <c r="D4" t="s">
+        <v>175</v>
+      </c>
+      <c r="E4" t="s">
+        <v>118</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="4" max="4" width="31.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="B1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="30">
+      <c r="A2" t="s">
+        <v>193</v>
+      </c>
+      <c r="B2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="E2" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="75">
+      <c r="A3" t="s">
+        <v>144</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="E3" t="s">
+        <v>118</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2688,8 +2820,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2782,8 +2914,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2845,12 +2977,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D38"/>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
+  <dimension ref="A1:D40"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32:B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2860,15 +2992,21 @@
     <col min="3" max="3" width="28.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>312</v>
       </c>
       <c r="B1" t="s">
         <v>313</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="C1" t="s">
+        <v>342</v>
+      </c>
+      <c r="D1" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>96</v>
       </c>
@@ -2879,7 +3017,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:4">
       <c r="A3" s="1" t="s">
         <v>92</v>
       </c>
@@ -2890,7 +3028,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:4">
       <c r="A4" s="1" t="s">
         <v>98</v>
       </c>
@@ -2901,7 +3039,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:4">
       <c r="A5" s="1" t="s">
         <v>93</v>
       </c>
@@ -2912,7 +3050,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:4">
       <c r="A6" s="1" t="s">
         <v>97</v>
       </c>
@@ -2923,7 +3061,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:4">
       <c r="A7" s="1" t="s">
         <v>97</v>
       </c>
@@ -2934,7 +3072,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:4">
       <c r="A8" s="1" t="s">
         <v>97</v>
       </c>
@@ -2945,7 +3083,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:4">
       <c r="A9" s="1" t="s">
         <v>97</v>
       </c>
@@ -2956,7 +3094,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:4">
       <c r="A10" s="1" t="s">
         <v>97</v>
       </c>
@@ -2967,7 +3105,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:4">
       <c r="A11" s="1" t="s">
         <v>97</v>
       </c>
@@ -2978,7 +3116,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:4">
       <c r="A12" s="1" t="s">
         <v>97</v>
       </c>
@@ -2989,7 +3127,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:4">
       <c r="A13" s="1" t="s">
         <v>94</v>
       </c>
@@ -3000,7 +3138,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:4">
       <c r="A14" s="1" t="s">
         <v>71</v>
       </c>
@@ -3011,7 +3149,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:4">
       <c r="A15" s="1" t="s">
         <v>95</v>
       </c>
@@ -3022,7 +3160,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:4">
       <c r="A16" s="1" t="s">
         <v>101</v>
       </c>
@@ -3194,59 +3332,81 @@
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="8" t="s">
+        <v>340</v>
+      </c>
+      <c r="B32" s="7" t="s">
+        <v>344</v>
+      </c>
+      <c r="D32" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="A33" s="8" t="s">
+        <v>341</v>
+      </c>
+      <c r="B33" s="7" t="s">
+        <v>345</v>
+      </c>
+      <c r="D33" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34" s="8" t="s">
         <v>279</v>
       </c>
-      <c r="B32" s="7" t="s">
+      <c r="B34" s="7" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="33" spans="1:3">
-      <c r="A33" s="8" t="s">
+    <row r="35" spans="1:4">
+      <c r="A35" s="8" t="s">
         <v>280</v>
       </c>
-      <c r="B33" s="7" t="s">
+      <c r="B35" s="7" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="34" spans="1:3">
-      <c r="A34" s="8" t="s">
+    <row r="36" spans="1:4">
+      <c r="A36" s="8" t="s">
         <v>281</v>
       </c>
-      <c r="B34" s="7" t="s">
+      <c r="B36" s="7" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="35" spans="1:3">
-      <c r="A35" s="8" t="s">
+    <row r="37" spans="1:4">
+      <c r="A37" s="8" t="s">
         <v>282</v>
       </c>
-      <c r="B35" s="7" t="s">
+      <c r="B37" s="7" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="36" spans="1:3">
-      <c r="A36" s="1" t="s">
+    <row r="38" spans="1:4">
+      <c r="A38" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="B36" s="7"/>
-      <c r="C36" t="s">
+      <c r="B38" s="7"/>
+      <c r="C38" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="37" spans="1:3">
-      <c r="A37" s="1" t="s">
+    <row r="39" spans="1:4">
+      <c r="A39" s="1" t="s">
         <v>283</v>
       </c>
-      <c r="B37" s="7"/>
-      <c r="C37" t="s">
+      <c r="B39" s="7"/>
+      <c r="C39" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="38" spans="1:3">
-      <c r="A38" s="1" t="s">
+    <row r="40" spans="1:4">
+      <c r="A40" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="B38" s="7"/>
+      <c r="B40" s="7"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:A1048576">
@@ -3260,8 +3420,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
   <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3412,8 +3572,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3496,8 +3656,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1900-000000000000}">
   <dimension ref="A1:D27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3853,8 +4013,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1A00-000000000000}">
   <dimension ref="A1:XFD14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -12171,8 +12331,65 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>200</v>
+      </c>
+      <c r="B3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" t="s">
+        <v>201</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1B00-000000000000}">
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -12264,68 +12481,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E3"/>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" t="s">
-        <v>200</v>
-      </c>
-      <c r="B3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" t="s">
-        <v>201</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E6"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
@@ -12425,7 +12585,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -12494,7 +12654,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -12585,7 +12745,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -12676,7 +12836,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -12742,7 +12902,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>